<commit_message>
refactor: remove supplier references from barang management
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\pwl-pos\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880E9175-BAC3-4301-8435-49AFF999363C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E25D4C-FF99-4522-9A00-645C158ADFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{760C5740-F267-4AB7-A48C-33505E437EB6}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8964" xr2:uid="{760C5740-F267-4AB7-A48C-33505E437EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>kategori_id</t>
-  </si>
-  <si>
-    <t>supplier_id</t>
   </si>
   <si>
     <t>barang_kode</t>
@@ -442,23 +439,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C426639B-0E22-441C-9A28-22ED8B83AD2C}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,107 +470,89 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
       </c>
       <c r="E2">
-        <v>10000</v>
-      </c>
-      <c r="F2">
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>40000</v>
       </c>
       <c r="E3">
-        <v>40000</v>
-      </c>
-      <c r="F3">
         <v>60000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>1000000</v>
       </c>
       <c r="E4">
-        <v>1000000</v>
-      </c>
-      <c r="F4">
         <v>2000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>2</v>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>4000000</v>
       </c>
       <c r="E5">
-        <v>4000000</v>
-      </c>
-      <c r="F5">
         <v>6000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>5000000</v>
       </c>
       <c r="E6">
-        <v>5000000</v>
-      </c>
-      <c r="F6">
         <v>7000000</v>
       </c>
     </row>

</xml_diff>